<commit_message>
still to be tuned up
</commit_message>
<xml_diff>
--- a/cleaned_data.xlsx
+++ b/cleaned_data.xlsx
@@ -458,7 +458,7 @@
         <v>125000</v>
       </c>
       <c r="D2" t="n">
-        <v>1970</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         <v>98000</v>
       </c>
       <c r="D3" t="n">
-        <v>1970</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>45000</v>
       </c>
       <c r="D4" t="n">
-        <v>1970</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>12000</v>
       </c>
       <c r="D5" t="n">
-        <v>1970</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         <v>28000</v>
       </c>
       <c r="D6" t="n">
-        <v>1970</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         <v>142000</v>
       </c>
       <c r="D7" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="8">
@@ -566,7 +566,7 @@
         <v>105000</v>
       </c>
       <c r="D8" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="9">
@@ -584,7 +584,7 @@
         <v>52000</v>
       </c>
       <c r="D9" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="10">
@@ -602,7 +602,7 @@
         <v>11500</v>
       </c>
       <c r="D10" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="11">
@@ -620,7 +620,7 @@
         <v>31000</v>
       </c>
       <c r="D11" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="12">
@@ -638,7 +638,7 @@
         <v>67000</v>
       </c>
       <c r="D12" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="13">
@@ -656,7 +656,7 @@
         <v>89000</v>
       </c>
       <c r="D13" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="14">
@@ -674,7 +674,7 @@
         <v>38000</v>
       </c>
       <c r="D14" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="15">
@@ -692,7 +692,7 @@
         <v>22000</v>
       </c>
       <c r="D15" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="16">
@@ -710,7 +710,7 @@
         <v>44000</v>
       </c>
       <c r="D16" t="n">
-        <v>1970</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="17">
@@ -728,7 +728,7 @@
         <v>158000</v>
       </c>
       <c r="D17" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="18">
@@ -746,7 +746,7 @@
         <v>112000</v>
       </c>
       <c r="D18" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="19">
@@ -764,7 +764,7 @@
         <v>61000</v>
       </c>
       <c r="D19" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="20">
@@ -782,7 +782,7 @@
         <v>13200</v>
       </c>
       <c r="D20" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="21">
@@ -800,7 +800,7 @@
         <v>34000</v>
       </c>
       <c r="D21" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="22">
@@ -818,7 +818,7 @@
         <v>73000</v>
       </c>
       <c r="D22" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="23">
@@ -836,7 +836,7 @@
         <v>95000</v>
       </c>
       <c r="D23" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="24">
@@ -854,7 +854,7 @@
         <v>44000</v>
       </c>
       <c r="D24" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="25">
@@ -872,7 +872,7 @@
         <v>26000</v>
       </c>
       <c r="D25" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="26">
@@ -890,7 +890,7 @@
         <v>51000</v>
       </c>
       <c r="D26" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="27">
@@ -908,7 +908,7 @@
         <v>41000</v>
       </c>
       <c r="D27" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="28">
@@ -926,7 +926,7 @@
         <v>78000</v>
       </c>
       <c r="D28" t="n">
-        <v>1970</v>
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>